<commit_message>
gak tau namain aapa
</commit_message>
<xml_diff>
--- a/Import/Inventories/product_category.xlsx
+++ b/Import/Inventories/product_category.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT Repositories\McDermott\Import\Inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E539F7-A6DB-4DE1-922E-1C4CF307E08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D665E6C-A6E2-400D-9FF3-0F1F23E8F26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,6 +31,7 @@
           <rPr>
             <sz val="11"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Mandatory</t>
         </r>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Name</t>
   </si>
@@ -347,13 +348,67 @@
   </si>
   <si>
     <t>PROD-050</t>
+  </si>
+  <si>
+    <t>Surgical Kits</t>
+  </si>
+  <si>
+    <t>Diagnostic Equipment</t>
+  </si>
+  <si>
+    <t>Fitness Equipment</t>
+  </si>
+  <si>
+    <t>Diagnostic Accessories</t>
+  </si>
+  <si>
+    <t>Patient Care Equipment</t>
+  </si>
+  <si>
+    <t>Hospital Accessories</t>
+  </si>
+  <si>
+    <t>Physiotherapy Equipment</t>
+  </si>
+  <si>
+    <t>Dialysis Equipment</t>
+  </si>
+  <si>
+    <t>Emergency Equipment</t>
+  </si>
+  <si>
+    <t>PROD-051</t>
+  </si>
+  <si>
+    <t>PROD-052</t>
+  </si>
+  <si>
+    <t>PROD-053</t>
+  </si>
+  <si>
+    <t>PROD-054</t>
+  </si>
+  <si>
+    <t>PROD-055</t>
+  </si>
+  <si>
+    <t>PROD-056</t>
+  </si>
+  <si>
+    <t>PROD-057</t>
+  </si>
+  <si>
+    <t>PROD-058</t>
+  </si>
+  <si>
+    <t>PROD-059</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -362,6 +417,17 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -399,12 +465,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,7 +490,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table" displayName="Table" ref="A1:B51" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table" displayName="Table" ref="A1:B60" headerRowCount="0">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Code"/>
@@ -729,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.6640625" defaultRowHeight="14.4"/>
@@ -1149,7 +1216,80 @@
         <v>101</v>
       </c>
     </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>